<commit_message>
Connected JDBC, created SQL, tested SQL
</commit_message>
<xml_diff>
--- a/App_Project_Lab_Details.xlsx
+++ b/App_Project_Lab_Details.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iamvi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Data Visualization for Lab Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B59ED16-538D-447E-A8A0-4C77DF91083C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7466B65C-25FA-4155-A5E7-99639E39D803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="7" xr2:uid="{124124BB-D469-4CEB-91E7-7C641825CE36}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="115">
   <si>
     <t>Complete Blood Test</t>
   </si>
@@ -58,9 +58,6 @@
     <t>ATTRIBUTE</t>
   </si>
   <si>
-    <t>YOUR RESULT</t>
-  </si>
-  <si>
     <t>NORMAL RANGE</t>
   </si>
   <si>
@@ -88,39 +85,21 @@
     <t>4.5 - 11.0</t>
   </si>
   <si>
-    <t>K/UL</t>
-  </si>
-  <si>
     <t>3.5 - 5.5</t>
   </si>
   <si>
-    <t>MIL/UL</t>
-  </si>
-  <si>
     <t>12.0 - 15.0</t>
   </si>
   <si>
-    <t>G/DL</t>
-  </si>
-  <si>
     <t>36.0 - 48.0</t>
   </si>
   <si>
-    <t>%</t>
-  </si>
-  <si>
     <t>79.0 - 101.0</t>
   </si>
   <si>
-    <t>FL</t>
-  </si>
-  <si>
     <t>25.0 - 35.0</t>
   </si>
   <si>
-    <t>PG</t>
-  </si>
-  <si>
     <t>31.0 - 37.0</t>
   </si>
   <si>
@@ -133,18 +112,12 @@
     <t>7.0 - 10.0</t>
   </si>
   <si>
-    <t>UNIT</t>
-  </si>
-  <si>
     <t>Urinalysis</t>
   </si>
   <si>
     <t>COLOR URINE</t>
   </si>
   <si>
-    <t>SPECIFIC GRAVITY URINE IRIS</t>
-  </si>
-  <si>
     <t>PH URINE</t>
   </si>
   <si>
@@ -166,18 +139,12 @@
     <t>CLEAR</t>
   </si>
   <si>
-    <t>1.001-1.035</t>
-  </si>
-  <si>
     <t>5.0-8.0</t>
   </si>
   <si>
     <t>NEGATIVE</t>
   </si>
   <si>
-    <t>APPEARANCE URINE</t>
-  </si>
-  <si>
     <t>GLUCOSE URINE IRIS</t>
   </si>
   <si>
@@ -187,9 +154,6 @@
     <t>BILIRUBIN URINE</t>
   </si>
   <si>
-    <t>&lt;2mg/dL</t>
-  </si>
-  <si>
     <t>T4</t>
   </si>
   <si>
@@ -208,12 +172,6 @@
     <t>0.5-5.0</t>
   </si>
   <si>
-    <t>pmol/L</t>
-  </si>
-  <si>
-    <t>mU/L</t>
-  </si>
-  <si>
     <t>Thyroid Test</t>
   </si>
   <si>
@@ -232,9 +190,6 @@
     <t>Less than 100</t>
   </si>
   <si>
-    <t>mg/dL</t>
-  </si>
-  <si>
     <t>Less than 140</t>
   </si>
   <si>
@@ -343,9 +298,6 @@
     <t>MARIJUANA METABOLITES</t>
   </si>
   <si>
-    <t>ng/mL</t>
-  </si>
-  <si>
     <t>Allergy Test</t>
   </si>
   <si>
@@ -391,10 +343,49 @@
     <t>Walnut</t>
   </si>
   <si>
-    <t>kU/L</t>
-  </si>
-  <si>
-    <t>&lt;0.10  [If more then that, then allergic]</t>
+    <t>Less than 2</t>
+  </si>
+  <si>
+    <t>Less than 0.10</t>
+  </si>
+  <si>
+    <t>Less than 0.11</t>
+  </si>
+  <si>
+    <t>Less than 0.12</t>
+  </si>
+  <si>
+    <t>Less than 0.13</t>
+  </si>
+  <si>
+    <t>Less than 0.14</t>
+  </si>
+  <si>
+    <t>Less than 0.15</t>
+  </si>
+  <si>
+    <t>Less than 0.16</t>
+  </si>
+  <si>
+    <t>Less than 0.17</t>
+  </si>
+  <si>
+    <t>Less than 0.18</t>
+  </si>
+  <si>
+    <t>Less than 0.19</t>
+  </si>
+  <si>
+    <t>Less than 0.20</t>
+  </si>
+  <si>
+    <t>Less than 0.21</t>
+  </si>
+  <si>
+    <t>Less than 0.22</t>
+  </si>
+  <si>
+    <t>Less than 0.23</t>
   </si>
 </sst>
 </file>
@@ -540,16 +531,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>138547</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>251112</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2130138</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>69271</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>294410</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>233795</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1220932</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>51954</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -571,7 +562,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10633365" y="796636"/>
+          <a:off x="2130138" y="4459431"/>
           <a:ext cx="4052454" cy="2866159"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -582,10 +573,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -885,148 +872,111 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A03B1932-8106-4738-BA8A-471C898EA36D}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="35.1328125" customWidth="1"/>
     <col min="2" max="2" width="20.53125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="24.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.59765625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.59765625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="35.65" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:3" ht="35.65" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="1" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="1" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="1" t="s">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="1" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1037,130 +987,113 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F915577E-84F5-4AB4-A0D0-F1DA37A72037}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
     <col min="2" max="2" width="25.1328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.19921875" customWidth="1"/>
-    <col min="4" max="4" width="21.796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.06640625" customWidth="1"/>
+    <col min="3" max="3" width="21.796875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.06640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" ht="34.9" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="34.9" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A1" s="4" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B1" s="5"/>
-      <c r="D1" s="5"/>
-    </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="C1" s="5"/>
+    </row>
+    <row r="2" spans="1:3" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C6" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C7" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B8" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B9" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+        <v>28</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+        <v>29</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1170,71 +1103,54 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B955421-BE90-41EB-AADB-0C5703D6306E}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="24.46484375" customWidth="1"/>
     <col min="2" max="2" width="23.19921875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.9296875" customWidth="1"/>
-    <col min="4" max="4" width="23.53125" customWidth="1"/>
-    <col min="5" max="5" width="15.53125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="25.5" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:3" ht="25.5" x14ac:dyDescent="0.75">
       <c r="A1" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B4" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B5" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>56</v>
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1244,71 +1160,54 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64F6D9BF-CC18-40D7-B988-0EBC74749FB6}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="36.73046875" customWidth="1"/>
     <col min="2" max="2" width="34.265625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.46484375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.46484375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A1" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B3" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+        <v>45</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+        <v>46</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B5" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>21</v>
+        <v>47</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1319,107 +1218,103 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{858E44FC-FB0F-427A-8EE1-9368FC2E4150}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="40.796875" style="4" customWidth="1"/>
     <col min="2" max="2" width="28.59765625" customWidth="1"/>
-    <col min="3" max="3" width="22.19921875" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" customWidth="1"/>
-    <col min="5" max="5" width="13.46484375" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A1" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.75">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.75">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.75">
+        <v>53</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.75">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.75">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B7" t="s">
-        <v>71</v>
-      </c>
-      <c r="D7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.75">
+        <v>56</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B8" t="s">
-        <v>72</v>
-      </c>
-      <c r="D8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.75">
+        <v>57</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.75">
+        <v>58</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B10" t="s">
-        <v>75</v>
-      </c>
-      <c r="D10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.75">
+        <v>60</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B11" t="s">
-        <v>74</v>
-      </c>
-      <c r="D11" t="s">
-        <v>43</v>
+        <v>59</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1430,104 +1325,78 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E3BB8DA-1816-4817-8CB2-4F3C68D9F0A2}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="26.33203125" style="4" customWidth="1"/>
     <col min="2" max="2" width="27" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.265625" customWidth="1"/>
-    <col min="4" max="4" width="30.796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.19921875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.796875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="42.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" ht="42.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B3" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="B4" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="B4" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="C4" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B5" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
+        <v>64</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B6" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.75">
+        <v>65</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B7" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.75">
+        <v>66</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B8" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1537,148 +1406,110 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BD87852-6E76-4B34-B2A7-FF09314B47D1}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="31.265625" style="4" customWidth="1"/>
     <col min="2" max="2" width="24.06640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.73046875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="26.86328125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.86328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A1" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B3" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D3" s="1">
+        <v>75</v>
+      </c>
+      <c r="C3" s="1">
         <v>1000</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B4" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D4" s="1">
+        <v>76</v>
+      </c>
+      <c r="C4" s="1">
         <v>300</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B5" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D5" s="1">
+        <v>77</v>
+      </c>
+      <c r="C5" s="1">
         <v>300</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B6" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D6" s="1">
+        <v>78</v>
+      </c>
+      <c r="C6" s="1">
         <v>300</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.75">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B7" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D7" s="1">
+        <v>84</v>
+      </c>
+      <c r="C7" s="1">
         <v>50</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.75">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B8" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D8" s="1">
+        <v>79</v>
+      </c>
+      <c r="C8" s="1">
         <v>300</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.75">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B9" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D9" s="1">
+        <v>80</v>
+      </c>
+      <c r="C9" s="1">
         <v>300</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.75">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B10" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D10" s="1">
+        <v>81</v>
+      </c>
+      <c r="C10" s="1">
         <v>300</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.75">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B11" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D11" s="1">
+        <v>82</v>
+      </c>
+      <c r="C11" s="1">
         <v>25</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.75">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B12" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D12" s="1">
+        <v>83</v>
+      </c>
+      <c r="C12" s="1">
         <v>300</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1688,192 +1519,142 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8295BFBA-26FE-49C0-8BFD-8AAF42070266}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="19.46484375" customWidth="1"/>
     <col min="2" max="2" width="19.59765625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.06640625" customWidth="1"/>
-    <col min="4" max="4" width="35.265625" customWidth="1"/>
-    <col min="5" max="5" width="13.06640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="35.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="25.5" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:3" ht="25.5" x14ac:dyDescent="0.75">
       <c r="A1" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" t="s">
         <v>102</v>
       </c>
-      <c r="D3" t="s">
-        <v>117</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B5" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" t="s">
         <v>103</v>
       </c>
-      <c r="D4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B5" s="1" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B6" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" t="s">
         <v>104</v>
       </c>
-      <c r="D5" t="s">
-        <v>117</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B6" s="1" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" t="s">
         <v>105</v>
       </c>
-      <c r="D6" t="s">
-        <v>117</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B7" s="1" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B8" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" t="s">
         <v>106</v>
       </c>
-      <c r="D7" t="s">
-        <v>117</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B8" s="1" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" t="s">
         <v>107</v>
       </c>
-      <c r="D8" t="s">
-        <v>117</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B9" s="1" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B10" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" t="s">
         <v>108</v>
       </c>
-      <c r="D9" t="s">
-        <v>117</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B10" s="1" t="s">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B11" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" t="s">
         <v>109</v>
       </c>
-      <c r="D10" t="s">
-        <v>117</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B11" s="1" t="s">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B12" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" t="s">
         <v>110</v>
       </c>
-      <c r="D11" t="s">
-        <v>117</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B12" s="1" t="s">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B13" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" t="s">
         <v>111</v>
       </c>
-      <c r="D12" t="s">
-        <v>117</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B13" s="1" t="s">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B14" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14" t="s">
         <v>112</v>
       </c>
-      <c r="D13" t="s">
-        <v>117</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B14" s="1" t="s">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B15" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" t="s">
         <v>113</v>
       </c>
-      <c r="D14" t="s">
-        <v>117</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B15" s="1" t="s">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B16" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" t="s">
         <v>114</v>
-      </c>
-      <c r="D15" t="s">
-        <v>117</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B16" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D16" t="s">
-        <v>117</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>